<commit_message>
Update de documentação metadados
</commit_message>
<xml_diff>
--- a/Documentos/Mapeamento das Fontes de Dados/VCOM/MAPEAMENTO_VCOM.xlsx
+++ b/Documentos/Mapeamento das Fontes de Dados/VCOM/MAPEAMENTO_VCOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\int.matheus\Desktop\DW\Data-Warehouse\Documentos\Mapeamento das Fontes de Dados\VCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066F02D7-9E65-467E-866E-22D479B1BF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF0C1A9-3639-446C-AA48-89375F1DD9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="787" firstSheet="3" activeTab="3" xr2:uid="{40AA39DE-57CF-4226-99BA-0B59FFBB7B19}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="787" firstSheet="3" activeTab="3" xr2:uid="{40AA39DE-57CF-4226-99BA-0B59FFBB7B19}"/>
   </bookViews>
   <sheets>
     <sheet name="PAINEL" sheetId="18" state="hidden" r:id="rId1"/>
@@ -1452,9 +1452,6 @@
     <t>ORIGEM CADASTRAL DO EMAIL</t>
   </si>
   <si>
-    <t>DADA DA CRIAÇÃO DO ACORDO</t>
-  </si>
-  <si>
     <t>USUARIO_ACORDO</t>
   </si>
   <si>
@@ -1640,6 +1637,9 @@
   </si>
   <si>
     <t>ID DO PAGAMENTO NO DW</t>
+  </si>
+  <si>
+    <t>DATA DA CRIAÇÃO DO ACORDO</t>
   </si>
 </sst>
 </file>
@@ -2588,7 +2588,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2648,10 +2648,10 @@
     </row>
     <row r="2" spans="1:13" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>420</v>
@@ -2677,7 +2677,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>462</v>
+        <v>517</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>422</v>
@@ -2890,22 +2890,22 @@
         <v>395</v>
       </c>
       <c r="I10" s="31" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K10" s="31" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L10" s="31"/>
     </row>
     <row r="11" spans="1:13" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="31" t="s">
+        <v>462</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>463</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>464</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>418</v>
@@ -2933,7 +2933,7 @@
         <v>42</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C12" s="31" t="s">
         <v>422</v>
@@ -2961,7 +2961,7 @@
         <v>41</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>422</v>
@@ -2986,10 +2986,10 @@
     </row>
     <row r="14" spans="1:13" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="31" t="s">
+        <v>466</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>467</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>468</v>
       </c>
       <c r="C14" s="31" t="s">
         <v>419</v>
@@ -3020,7 +3020,7 @@
         <v>242</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D15" s="31">
         <v>9.1999999999999993</v>
@@ -3102,7 +3102,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:J17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.33203125" defaultRowHeight="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3161,10 +3161,10 @@
     </row>
     <row r="2" spans="1:12" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>420</v>
@@ -3209,10 +3209,10 @@
         <v>395</v>
       </c>
       <c r="I3" s="31" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="J3" s="31" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K3" s="31"/>
       <c r="L3" s="31"/>
@@ -3407,22 +3407,22 @@
         <v>395</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="J10" s="29" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L10" s="31"/>
     </row>
     <row r="11" spans="1:12" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="31" t="s">
+        <v>469</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>470</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>471</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>418</v>
@@ -3441,13 +3441,13 @@
         <v>395</v>
       </c>
       <c r="I11" s="31" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="J11" s="31" t="s">
+        <v>506</v>
+      </c>
+      <c r="K11" s="31" t="s">
         <v>507</v>
-      </c>
-      <c r="K11" s="31" t="s">
-        <v>508</v>
       </c>
       <c r="L11" s="31"/>
     </row>
@@ -3456,7 +3456,7 @@
         <v>48</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C12" s="31" t="s">
         <v>418</v>
@@ -3475,22 +3475,22 @@
         <v>395</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="J12" s="31" t="s">
+        <v>506</v>
+      </c>
+      <c r="K12" s="31" t="s">
         <v>507</v>
-      </c>
-      <c r="K12" s="31" t="s">
-        <v>508</v>
       </c>
       <c r="L12" s="31"/>
     </row>
     <row r="13" spans="1:12" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="31" t="s">
+        <v>472</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>473</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>474</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>419</v>
@@ -3509,20 +3509,20 @@
         <v>395</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
     </row>
     <row r="14" spans="1:12" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="31" t="s">
+        <v>474</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>475</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>476</v>
       </c>
       <c r="C14" s="31" t="s">
         <v>418</v>
@@ -3541,13 +3541,13 @@
         <v>395</v>
       </c>
       <c r="I14" s="31" t="s">
+        <v>501</v>
+      </c>
+      <c r="J14" s="31" t="s">
         <v>502</v>
       </c>
-      <c r="J14" s="31" t="s">
+      <c r="K14" s="31" t="s">
         <v>503</v>
-      </c>
-      <c r="K14" s="31" t="s">
-        <v>504</v>
       </c>
       <c r="L14" s="31"/>
     </row>
@@ -3559,7 +3559,7 @@
         <v>243</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D15" s="31">
         <v>9.1999999999999993</v>
@@ -3575,10 +3575,10 @@
         <v>395</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="J15" s="31" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K15" s="31"/>
       <c r="L15" s="31"/>
@@ -3716,7 +3716,7 @@
         <v>330</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -7479,7 +7479,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F21" sqref="F21:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="22.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7542,10 +7542,10 @@
     </row>
     <row r="2" spans="1:13" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B2" s="31" t="s">
         <v>512</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>513</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>420</v>
@@ -8257,7 +8257,7 @@
       <c r="K2" s="31"/>
       <c r="L2" s="31"/>
       <c r="M2" s="46" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8320,7 +8320,7 @@
         <v>404</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K4" s="31"/>
       <c r="L4" s="31"/>
@@ -8493,13 +8493,13 @@
         <v>395</v>
       </c>
       <c r="I10" s="31" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K10" s="31" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L10" s="31"/>
       <c r="M10" s="46"/>
@@ -8531,7 +8531,7 @@
         <v>404</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
@@ -8561,13 +8561,13 @@
         <v>395</v>
       </c>
       <c r="I12" s="31" t="s">
+        <v>487</v>
+      </c>
+      <c r="J12" s="31" t="s">
         <v>488</v>
       </c>
-      <c r="J12" s="31" t="s">
-        <v>489</v>
-      </c>
       <c r="K12" s="31" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="L12" s="31"/>
       <c r="M12" s="46"/>
@@ -8599,7 +8599,7 @@
         <v>404</v>
       </c>
       <c r="J13" s="41" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
@@ -8631,13 +8631,13 @@
         <v>395</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K14" s="31" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L14" s="31"/>
       <c r="M14" s="46"/>
@@ -8853,7 +8853,7 @@
       <c r="K2" s="31"/>
       <c r="L2" s="31"/>
       <c r="M2" s="49" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8880,7 +8880,7 @@
         <v>395</v>
       </c>
       <c r="I3" s="31" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J3" s="31" t="s">
         <v>409</v>
@@ -8894,7 +8894,7 @@
         <v>439</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C4" s="31" t="s">
         <v>422</v>
@@ -8913,10 +8913,10 @@
         <v>395</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K4" s="31"/>
       <c r="L4" s="31"/>
@@ -9089,13 +9089,13 @@
         <v>395</v>
       </c>
       <c r="I10" s="31" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K10" s="31" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L10" s="31"/>
       <c r="M10" s="50"/>
@@ -9124,14 +9124,14 @@
         <v>395</v>
       </c>
       <c r="I11" s="31" t="s">
+        <v>489</v>
+      </c>
+      <c r="J11" s="31" t="s">
         <v>490</v>
-      </c>
-      <c r="J11" s="31" t="s">
-        <v>491</v>
       </c>
       <c r="K11" s="31"/>
       <c r="L11" s="31" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="M11" s="50"/>
     </row>
@@ -9149,7 +9149,7 @@
         <v>30</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F12" s="31" t="s">
         <v>393</v>
@@ -9161,13 +9161,13 @@
         <v>395</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J12" s="31" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K12" s="31" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L12" s="31"/>
       <c r="M12" s="50"/>
@@ -9198,13 +9198,13 @@
         <v>395</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K13" s="31" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L13" s="31"/>
       <c r="M13" s="50"/>
@@ -9233,10 +9233,10 @@
         <v>395</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>

</xml_diff>